<commit_message>
Updated litter chemistry data
Ashish messed up column headings in the original litter chemistry data. So he sent in new files with the column headings fixed. Also sent in a powerpoint describing the functional groups, too.
</commit_message>
<xml_diff>
--- a/Litter chemistry/ftir.percent.area_brian.xlsx
+++ b/Litter chemistry/ftir.percent.area_brian.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s18am9/Documents/UCI/FTIR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08D012C-D183-6244-BEC9-0CC64438CF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA44E458-E4F6-304F-9E65-AE3520158B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20620" yWindow="2880" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftir.percent.area_2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ftir.percent.area_2!$D$2:$D$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ftir.percent.area_2!$D$1:$D$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -275,27 +275,6 @@
   </si>
   <si>
     <t>T4</t>
-  </si>
-  <si>
-    <t>Carbohydrate: ester bonds</t>
-  </si>
-  <si>
-    <t>Carbohydrate: glycosidic bonds</t>
-  </si>
-  <si>
-    <t>Carbohydrate: C-O stretching</t>
-  </si>
-  <si>
-    <t>Aliphatic like alkane: C-H bending</t>
-  </si>
-  <si>
-    <t>Protein (amide 2): N-H bending</t>
-  </si>
-  <si>
-    <t>Protein (amide 1): N-H bending</t>
-  </si>
-  <si>
-    <t>Lipid (aldehyde or ester): C=O stretching</t>
   </si>
 </sst>
 </file>
@@ -1143,271 +1122,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>7.7681350990000002</v>
+      </c>
+      <c r="F2">
+        <v>13.77563761</v>
+      </c>
+      <c r="G2">
+        <v>6.3511344909999998</v>
+      </c>
+      <c r="H2">
+        <v>3.8925087939999998</v>
+      </c>
+      <c r="I2">
+        <v>1.1230756120000001</v>
+      </c>
+      <c r="J2">
+        <v>2.2384544000000002</v>
+      </c>
+      <c r="K2">
+        <v>1.335423284</v>
+      </c>
+      <c r="L2">
+        <v>1.134422987</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E3">
-        <v>7.7681350990000002</v>
+        <v>6.561219812</v>
       </c>
       <c r="F3">
-        <v>13.77563761</v>
+        <v>11.53335631</v>
       </c>
       <c r="G3">
-        <v>6.3511344909999998</v>
+        <v>5.9592366940000003</v>
       </c>
       <c r="H3">
-        <v>3.8925087939999998</v>
+        <v>4.5260622670000004</v>
       </c>
       <c r="I3">
-        <v>1.1230756120000001</v>
+        <v>1.388816676</v>
       </c>
       <c r="J3">
-        <v>2.2384544000000002</v>
+        <v>3.0147903060000001</v>
       </c>
       <c r="K3">
-        <v>1.335423284</v>
+        <v>1.7823717370000001</v>
       </c>
       <c r="L3">
-        <v>1.134422987</v>
+        <v>1.4710161429999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4">
-        <v>6.561219812</v>
+        <v>5.2755822749999997</v>
       </c>
       <c r="F4">
-        <v>11.53335631</v>
+        <v>9.1564917589999997</v>
       </c>
       <c r="G4">
-        <v>5.9592366940000003</v>
+        <v>5.424979875</v>
       </c>
       <c r="H4">
-        <v>4.5260622670000004</v>
+        <v>4.4283433069999996</v>
       </c>
       <c r="I4">
-        <v>1.388816676</v>
+        <v>1.646435155</v>
       </c>
       <c r="J4">
-        <v>3.0147903060000001</v>
+        <v>4.2384880359999997</v>
       </c>
       <c r="K4">
-        <v>1.7823717370000001</v>
+        <v>2.1446158369999999</v>
       </c>
       <c r="L4">
-        <v>1.4710161429999999</v>
+        <v>2.2020501449999998</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E5">
-        <v>5.2755822749999997</v>
+        <v>6.4161242280000002</v>
       </c>
       <c r="F5">
-        <v>9.1564917589999997</v>
+        <v>10.28824528</v>
       </c>
       <c r="G5">
-        <v>5.424979875</v>
+        <v>5.9161351590000004</v>
       </c>
       <c r="H5">
-        <v>4.4283433069999996</v>
+        <v>4.8777136189999997</v>
       </c>
       <c r="I5">
-        <v>1.646435155</v>
+        <v>1.44298623</v>
       </c>
       <c r="J5">
-        <v>4.2384880359999997</v>
+        <v>3.3424136249999998</v>
       </c>
       <c r="K5">
-        <v>2.1446158369999999</v>
+        <v>1.946441104</v>
       </c>
       <c r="L5">
-        <v>2.2020501449999998</v>
+        <v>1.4684125720000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E6">
-        <v>6.4161242280000002</v>
+        <v>4.6066318119999998</v>
       </c>
       <c r="F6">
-        <v>10.28824528</v>
+        <v>7.2780192460000004</v>
       </c>
       <c r="G6">
-        <v>5.9161351590000004</v>
+        <v>5.4208096320000001</v>
       </c>
       <c r="H6">
-        <v>4.8777136189999997</v>
+        <v>6.4253014400000001</v>
       </c>
       <c r="I6">
-        <v>1.44298623</v>
+        <v>2.1008396130000002</v>
       </c>
       <c r="J6">
-        <v>3.3424136249999998</v>
+        <v>3.3286088839999999</v>
       </c>
       <c r="K6">
-        <v>1.946441104</v>
+        <v>1.959190397</v>
       </c>
       <c r="L6">
-        <v>1.4684125720000001</v>
+        <v>3.7066430659999998</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>78</v>
       </c>
       <c r="E7">
-        <v>4.6066318119999998</v>
+        <v>4.4554788829999996</v>
       </c>
       <c r="F7">
-        <v>7.2780192460000004</v>
+        <v>7.1016887029999998</v>
       </c>
       <c r="G7">
-        <v>5.4208096320000001</v>
+        <v>5.6415356809999997</v>
       </c>
       <c r="H7">
-        <v>6.4253014400000001</v>
+        <v>6.1016956960000002</v>
       </c>
       <c r="I7">
-        <v>2.1008396130000002</v>
+        <v>3.270740462</v>
       </c>
       <c r="J7">
-        <v>3.3286088839999999</v>
+        <v>2.6648320640000001</v>
       </c>
       <c r="K7">
-        <v>1.959190397</v>
+        <v>1.6784396349999999</v>
       </c>
       <c r="L7">
-        <v>3.7066430659999998</v>
+        <v>4.1629552780000001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>80</v>
@@ -1419,299 +1410,299 @@
         <v>78</v>
       </c>
       <c r="E8">
-        <v>4.4554788829999996</v>
+        <v>4.4029166420000001</v>
       </c>
       <c r="F8">
-        <v>7.1016887029999998</v>
+        <v>6.8270798739999998</v>
       </c>
       <c r="G8">
-        <v>5.6415356809999997</v>
+        <v>5.2482446810000001</v>
       </c>
       <c r="H8">
-        <v>6.1016956960000002</v>
+        <v>6.7692193869999997</v>
       </c>
       <c r="I8">
-        <v>3.270740462</v>
+        <v>2.310079746</v>
       </c>
       <c r="J8">
-        <v>2.6648320640000001</v>
+        <v>2.9049542019999999</v>
       </c>
       <c r="K8">
-        <v>1.6784396349999999</v>
+        <v>1.7640803410000001</v>
       </c>
       <c r="L8">
-        <v>4.1629552780000001</v>
+        <v>4.7558366940000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>78</v>
       </c>
       <c r="E9">
-        <v>4.4029166420000001</v>
+        <v>4.5292374569999998</v>
       </c>
       <c r="F9">
-        <v>6.8270798739999998</v>
+        <v>6.9062411099999998</v>
       </c>
       <c r="G9">
-        <v>5.2482446810000001</v>
+        <v>5.369364987</v>
       </c>
       <c r="H9">
-        <v>6.7692193869999997</v>
+        <v>6.5184661850000003</v>
       </c>
       <c r="I9">
-        <v>2.310079746</v>
+        <v>2.3784479379999999</v>
       </c>
       <c r="J9">
-        <v>2.9049542019999999</v>
+        <v>3.1038322420000002</v>
       </c>
       <c r="K9">
-        <v>1.7640803410000001</v>
+        <v>1.8615891010000001</v>
       </c>
       <c r="L9">
-        <v>4.7558366940000001</v>
+        <v>3.9019419200000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E10">
-        <v>4.5292374569999998</v>
+        <v>6.5054797689999999</v>
       </c>
       <c r="F10">
-        <v>6.9062411099999998</v>
+        <v>11.710607830000001</v>
       </c>
       <c r="G10">
-        <v>5.369364987</v>
+        <v>6.7791945589999996</v>
       </c>
       <c r="H10">
-        <v>6.5184661850000003</v>
+        <v>5.54467161</v>
       </c>
       <c r="I10">
-        <v>2.3784479379999999</v>
+        <v>1.1294257560000001</v>
       </c>
       <c r="J10">
-        <v>3.1038322420000002</v>
+        <v>2.3691010339999998</v>
       </c>
       <c r="K10">
-        <v>1.8615891010000001</v>
+        <v>1.47925591</v>
       </c>
       <c r="L10">
-        <v>3.9019419200000001</v>
+        <v>1.9706376299999999</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11">
-        <v>6.5054797689999999</v>
+        <v>4.6107767519999996</v>
       </c>
       <c r="F11">
-        <v>11.710607830000001</v>
+        <v>6.9279388370000001</v>
       </c>
       <c r="G11">
-        <v>6.7791945589999996</v>
+        <v>5.8058653639999998</v>
       </c>
       <c r="H11">
-        <v>5.54467161</v>
+        <v>6.4454190789999997</v>
       </c>
       <c r="I11">
-        <v>1.1294257560000001</v>
+        <v>3.2069415430000001</v>
       </c>
       <c r="J11">
-        <v>2.3691010339999998</v>
+        <v>2.267328708</v>
       </c>
       <c r="K11">
-        <v>1.47925591</v>
+        <v>1.391932293</v>
       </c>
       <c r="L11">
-        <v>1.9706376299999999</v>
+        <v>4.8560015520000004</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>78</v>
       </c>
       <c r="E12">
-        <v>4.6107767519999996</v>
+        <v>5.0046699739999996</v>
       </c>
       <c r="F12">
-        <v>6.9279388370000001</v>
+        <v>7.42397054</v>
       </c>
       <c r="G12">
-        <v>5.8058653639999998</v>
+        <v>4.9797780820000002</v>
       </c>
       <c r="H12">
-        <v>6.4454190789999997</v>
+        <v>5.9233672769999997</v>
       </c>
       <c r="I12">
-        <v>3.2069415430000001</v>
+        <v>1.991165383</v>
       </c>
       <c r="J12">
-        <v>2.267328708</v>
+        <v>3.538878709</v>
       </c>
       <c r="K12">
-        <v>1.391932293</v>
+        <v>1.921991386</v>
       </c>
       <c r="L12">
-        <v>4.8560015520000004</v>
+        <v>3.6433407029999998</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>78</v>
       </c>
       <c r="E13">
-        <v>5.0046699739999996</v>
+        <v>5.080564807</v>
       </c>
       <c r="F13">
-        <v>7.42397054</v>
+        <v>7.698227674</v>
       </c>
       <c r="G13">
-        <v>4.9797780820000002</v>
+        <v>5.2893300869999997</v>
       </c>
       <c r="H13">
-        <v>5.9233672769999997</v>
+        <v>6.3051963400000002</v>
       </c>
       <c r="I13">
-        <v>1.991165383</v>
+        <v>1.806968184</v>
       </c>
       <c r="J13">
-        <v>3.538878709</v>
+        <v>3.3291418560000001</v>
       </c>
       <c r="K13">
-        <v>1.921991386</v>
+        <v>1.878423889</v>
       </c>
       <c r="L13">
-        <v>3.6433407029999998</v>
+        <v>3.5407503010000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
         <v>78</v>
       </c>
       <c r="E14">
-        <v>5.080564807</v>
+        <v>4.9203799789999998</v>
       </c>
       <c r="F14">
-        <v>7.698227674</v>
+        <v>7.6511202630000001</v>
       </c>
       <c r="G14">
-        <v>5.2893300869999997</v>
+        <v>5.38019508</v>
       </c>
       <c r="H14">
-        <v>6.3051963400000002</v>
+        <v>5.9353290339999996</v>
       </c>
       <c r="I14">
-        <v>1.806968184</v>
+        <v>2.5736815229999999</v>
       </c>
       <c r="J14">
-        <v>3.3291418560000001</v>
+        <v>2.9485770790000001</v>
       </c>
       <c r="K14">
-        <v>1.878423889</v>
+        <v>1.7932857390000001</v>
       </c>
       <c r="L14">
-        <v>3.5407503010000001</v>
+        <v>4.1297173010000003</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>78</v>
       </c>
       <c r="E15">
-        <v>4.9203799789999998</v>
+        <v>6.7348817749999998</v>
       </c>
       <c r="F15">
-        <v>7.6511202630000001</v>
+        <v>12.00766701</v>
       </c>
       <c r="G15">
-        <v>5.38019508</v>
+        <v>6.9240585049999996</v>
       </c>
       <c r="H15">
-        <v>5.9353290339999996</v>
+        <v>5.4838680860000002</v>
       </c>
       <c r="I15">
-        <v>2.5736815229999999</v>
+        <v>1.0549117649999999</v>
       </c>
       <c r="J15">
-        <v>2.9485770790000001</v>
+        <v>2.5777758149999999</v>
       </c>
       <c r="K15">
-        <v>1.7932857390000001</v>
+        <v>1.573318349</v>
       </c>
       <c r="L15">
-        <v>4.1297173010000003</v>
+        <v>1.248208022</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>76</v>
@@ -1723,299 +1714,299 @@
         <v>78</v>
       </c>
       <c r="E16">
-        <v>6.7348817749999998</v>
+        <v>5.6045706160000002</v>
       </c>
       <c r="F16">
-        <v>12.00766701</v>
+        <v>8.1490614679999993</v>
       </c>
       <c r="G16">
-        <v>6.9240585049999996</v>
+        <v>4.7416525089999997</v>
       </c>
       <c r="H16">
-        <v>5.4838680860000002</v>
+        <v>4.2475088029999997</v>
       </c>
       <c r="I16">
-        <v>1.0549117649999999</v>
+        <v>1.6391300310000001</v>
       </c>
       <c r="J16">
-        <v>2.5777758149999999</v>
+        <v>5.1161346200000004</v>
       </c>
       <c r="K16">
-        <v>1.573318349</v>
+        <v>2.348569387</v>
       </c>
       <c r="L16">
-        <v>1.248208022</v>
+        <v>2.4625343370000001</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E17">
-        <v>5.6045706160000002</v>
+        <v>6.7495423910000003</v>
       </c>
       <c r="F17">
-        <v>8.1490614679999993</v>
+        <v>12.659985860000001</v>
       </c>
       <c r="G17">
-        <v>4.7416525089999997</v>
+        <v>6.7642927850000003</v>
       </c>
       <c r="H17">
-        <v>4.2475088029999997</v>
+        <v>5.2296281369999997</v>
       </c>
       <c r="I17">
-        <v>1.6391300310000001</v>
+        <v>1.1062482419999999</v>
       </c>
       <c r="J17">
-        <v>5.1161346200000004</v>
+        <v>2.200549364</v>
       </c>
       <c r="K17">
-        <v>2.348569387</v>
+        <v>1.480005797</v>
       </c>
       <c r="L17">
-        <v>2.4625343370000001</v>
+        <v>1.3990453709999999</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>81</v>
       </c>
       <c r="E18">
-        <v>6.7495423910000003</v>
+        <v>8.1817139950000008</v>
       </c>
       <c r="F18">
-        <v>12.659985860000001</v>
+        <v>13.10715334</v>
       </c>
       <c r="G18">
-        <v>6.7642927850000003</v>
+        <v>5.7533917109999999</v>
       </c>
       <c r="H18">
-        <v>5.2296281369999997</v>
+        <v>3.5202274980000001</v>
       </c>
       <c r="I18">
-        <v>1.1062482419999999</v>
+        <v>1.277696589</v>
       </c>
       <c r="J18">
-        <v>2.200549364</v>
+        <v>2.4826327410000002</v>
       </c>
       <c r="K18">
-        <v>1.480005797</v>
+        <v>1.485376582</v>
       </c>
       <c r="L18">
-        <v>1.3990453709999999</v>
+        <v>1.128930502</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E19">
-        <v>8.1817139950000008</v>
+        <v>6.7059387539999999</v>
       </c>
       <c r="F19">
-        <v>13.10715334</v>
+        <v>12.51412264</v>
       </c>
       <c r="G19">
-        <v>5.7533917109999999</v>
+        <v>6.9161628789999998</v>
       </c>
       <c r="H19">
-        <v>3.5202274980000001</v>
+        <v>5.4382446729999998</v>
       </c>
       <c r="I19">
-        <v>1.277696589</v>
+        <v>1.0647773309999999</v>
       </c>
       <c r="J19">
-        <v>2.4826327410000002</v>
+        <v>2.3331465040000001</v>
       </c>
       <c r="K19">
-        <v>1.485376582</v>
+        <v>1.3737068370000001</v>
       </c>
       <c r="L19">
-        <v>1.128930502</v>
+        <v>1.4306772290000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E20">
-        <v>6.7059387539999999</v>
+        <v>7.7671174650000001</v>
       </c>
       <c r="F20">
-        <v>12.51412264</v>
+        <v>11.690420169999999</v>
       </c>
       <c r="G20">
-        <v>6.9161628789999998</v>
+        <v>6.1550716230000004</v>
       </c>
       <c r="H20">
-        <v>5.4382446729999998</v>
+        <v>4.6160691619999996</v>
       </c>
       <c r="I20">
-        <v>1.0647773309999999</v>
+        <v>1.095190179</v>
       </c>
       <c r="J20">
-        <v>2.3331465040000001</v>
+        <v>2.5859904600000001</v>
       </c>
       <c r="K20">
-        <v>1.3737068370000001</v>
+        <v>1.576821528</v>
       </c>
       <c r="L20">
-        <v>1.4306772290000001</v>
+        <v>1.952938345</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E21">
-        <v>7.7671174650000001</v>
+        <v>7.3780710239999996</v>
       </c>
       <c r="F21">
-        <v>11.690420169999999</v>
+        <v>12.60641875</v>
       </c>
       <c r="G21">
-        <v>6.1550716230000004</v>
+        <v>5.9565906369999997</v>
       </c>
       <c r="H21">
-        <v>4.6160691619999996</v>
+        <v>3.9673231420000001</v>
       </c>
       <c r="I21">
-        <v>1.095190179</v>
+        <v>1.243225928</v>
       </c>
       <c r="J21">
-        <v>2.5859904600000001</v>
+        <v>2.4413969409999998</v>
       </c>
       <c r="K21">
-        <v>1.576821528</v>
+        <v>1.5149423829999999</v>
       </c>
       <c r="L21">
-        <v>1.952938345</v>
+        <v>1.467390191</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E22">
-        <v>7.3780710239999996</v>
+        <v>4.9714848600000003</v>
       </c>
       <c r="F22">
-        <v>12.60641875</v>
+        <v>7.5066787670000004</v>
       </c>
       <c r="G22">
-        <v>5.9565906369999997</v>
+        <v>5.189492757</v>
       </c>
       <c r="H22">
-        <v>3.9673231420000001</v>
+        <v>5.8038269659999999</v>
       </c>
       <c r="I22">
-        <v>1.243225928</v>
+        <v>2.1991900750000002</v>
       </c>
       <c r="J22">
-        <v>2.4413969409999998</v>
+        <v>3.262230449</v>
       </c>
       <c r="K22">
-        <v>1.5149423829999999</v>
+        <v>1.922578296</v>
       </c>
       <c r="L22">
-        <v>1.467390191</v>
+        <v>3.783220112</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
         <v>81</v>
       </c>
       <c r="E23">
-        <v>4.9714848600000003</v>
+        <v>4.8151962880000001</v>
       </c>
       <c r="F23">
-        <v>7.5066787670000004</v>
+        <v>7.7058545379999996</v>
       </c>
       <c r="G23">
-        <v>5.189492757</v>
+        <v>5.1189766880000001</v>
       </c>
       <c r="H23">
-        <v>5.8038269659999999</v>
+        <v>5.6339923430000001</v>
       </c>
       <c r="I23">
-        <v>2.1991900750000002</v>
+        <v>2.1746107609999998</v>
       </c>
       <c r="J23">
-        <v>3.262230449</v>
+        <v>3.5120593599999999</v>
       </c>
       <c r="K23">
-        <v>1.922578296</v>
+        <v>2.1193621299999998</v>
       </c>
       <c r="L23">
-        <v>3.783220112</v>
+        <v>3.5885142440000002</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>80</v>
@@ -2027,299 +2018,299 @@
         <v>81</v>
       </c>
       <c r="E24">
-        <v>4.8151962880000001</v>
+        <v>4.3459253379999998</v>
       </c>
       <c r="F24">
-        <v>7.7058545379999996</v>
+        <v>6.6079708720000001</v>
       </c>
       <c r="G24">
-        <v>5.1189766880000001</v>
+        <v>5.2560076489999998</v>
       </c>
       <c r="H24">
-        <v>5.6339923430000001</v>
+        <v>6.4774573369999997</v>
       </c>
       <c r="I24">
-        <v>2.1746107609999998</v>
+        <v>2.2497172249999999</v>
       </c>
       <c r="J24">
-        <v>3.5120593599999999</v>
+        <v>2.9958658460000001</v>
       </c>
       <c r="K24">
-        <v>2.1193621299999998</v>
+        <v>1.784904756</v>
       </c>
       <c r="L24">
-        <v>3.5885142440000002</v>
+        <v>5.2340367140000001</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>81</v>
       </c>
       <c r="E25">
-        <v>4.3459253379999998</v>
+        <v>4.9380096379999996</v>
       </c>
       <c r="F25">
-        <v>6.6079708720000001</v>
+        <v>7.5309125100000003</v>
       </c>
       <c r="G25">
-        <v>5.2560076489999998</v>
+        <v>5.1387284160000002</v>
       </c>
       <c r="H25">
-        <v>6.4774573369999997</v>
+        <v>5.850841001</v>
       </c>
       <c r="I25">
-        <v>2.2497172249999999</v>
+        <v>2.013497111</v>
       </c>
       <c r="J25">
-        <v>2.9958658460000001</v>
+        <v>3.5266035379999998</v>
       </c>
       <c r="K25">
-        <v>1.784904756</v>
+        <v>2.0998494289999998</v>
       </c>
       <c r="L25">
-        <v>5.2340367140000001</v>
+        <v>3.5070528030000001</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E26">
-        <v>4.9380096379999996</v>
+        <v>7.3901249780000002</v>
       </c>
       <c r="F26">
-        <v>7.5309125100000003</v>
+        <v>11.459704110000001</v>
       </c>
       <c r="G26">
-        <v>5.1387284160000002</v>
+        <v>5.7256707660000004</v>
       </c>
       <c r="H26">
-        <v>5.850841001</v>
+        <v>4.0565346709999996</v>
       </c>
       <c r="I26">
-        <v>2.013497111</v>
+        <v>1.312239513</v>
       </c>
       <c r="J26">
-        <v>3.5266035379999998</v>
+        <v>2.8551382159999998</v>
       </c>
       <c r="K26">
-        <v>2.0998494289999998</v>
+        <v>1.60754061</v>
       </c>
       <c r="L26">
-        <v>3.5070528030000001</v>
+        <v>1.8039439530000001</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E27">
-        <v>7.3901249780000002</v>
+        <v>4.5196135789999996</v>
       </c>
       <c r="F27">
-        <v>11.459704110000001</v>
+        <v>7.2172661700000003</v>
       </c>
       <c r="G27">
-        <v>5.7256707660000004</v>
+        <v>4.8068200660000002</v>
       </c>
       <c r="H27">
-        <v>4.0565346709999996</v>
+        <v>5.032958539</v>
       </c>
       <c r="I27">
-        <v>1.312239513</v>
+        <v>1.809411592</v>
       </c>
       <c r="J27">
-        <v>2.8551382159999998</v>
+        <v>4.7300269410000002</v>
       </c>
       <c r="K27">
-        <v>1.60754061</v>
+        <v>2.6611858349999999</v>
       </c>
       <c r="L27">
-        <v>1.8039439530000001</v>
+        <v>2.9655760440000001</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
         <v>81</v>
       </c>
       <c r="E28">
-        <v>4.5196135789999996</v>
+        <v>4.3635068390000002</v>
       </c>
       <c r="F28">
-        <v>7.2172661700000003</v>
+        <v>6.8676216170000002</v>
       </c>
       <c r="G28">
-        <v>4.8068200660000002</v>
+        <v>5.294061074</v>
       </c>
       <c r="H28">
-        <v>5.032958539</v>
+        <v>7.1142020060000002</v>
       </c>
       <c r="I28">
-        <v>1.809411592</v>
+        <v>1.921017159</v>
       </c>
       <c r="J28">
-        <v>4.7300269410000002</v>
+        <v>3.019023829</v>
       </c>
       <c r="K28">
-        <v>2.6611858349999999</v>
+        <v>1.8368795449999999</v>
       </c>
       <c r="L28">
-        <v>2.9655760440000001</v>
+        <v>4.4663026180000003</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
         <v>81</v>
       </c>
       <c r="E29">
-        <v>4.3635068390000002</v>
+        <v>4.369436973</v>
       </c>
       <c r="F29">
-        <v>6.8676216170000002</v>
+        <v>7.070031986</v>
       </c>
       <c r="G29">
-        <v>5.294061074</v>
+        <v>5.3064807810000003</v>
       </c>
       <c r="H29">
-        <v>7.1142020060000002</v>
+        <v>6.159781304</v>
       </c>
       <c r="I29">
-        <v>1.921017159</v>
+        <v>2.287166848</v>
       </c>
       <c r="J29">
-        <v>3.019023829</v>
+        <v>3.2748590320000002</v>
       </c>
       <c r="K29">
-        <v>1.8368795449999999</v>
+        <v>1.987461554</v>
       </c>
       <c r="L29">
-        <v>4.4663026180000003</v>
+        <v>4.0050468199999996</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
         <v>81</v>
       </c>
       <c r="E30">
-        <v>4.369436973</v>
+        <v>4.5526754829999998</v>
       </c>
       <c r="F30">
-        <v>7.070031986</v>
+        <v>7.1293986089999999</v>
       </c>
       <c r="G30">
-        <v>5.3064807810000003</v>
+        <v>5.5351800420000004</v>
       </c>
       <c r="H30">
-        <v>6.159781304</v>
+        <v>6.509377282</v>
       </c>
       <c r="I30">
-        <v>2.287166848</v>
+        <v>2.349909851</v>
       </c>
       <c r="J30">
-        <v>3.2748590320000002</v>
+        <v>2.916987491</v>
       </c>
       <c r="K30">
-        <v>1.987461554</v>
+        <v>1.7118722850000001</v>
       </c>
       <c r="L30">
-        <v>4.0050468199999996</v>
+        <v>4.5414139169999999</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
         <v>81</v>
       </c>
       <c r="E31">
-        <v>4.5526754829999998</v>
+        <v>4.1500677860000001</v>
       </c>
       <c r="F31">
-        <v>7.1293986089999999</v>
+        <v>7.21392773</v>
       </c>
       <c r="G31">
-        <v>5.5351800420000004</v>
+        <v>4.636718525</v>
       </c>
       <c r="H31">
-        <v>6.509377282</v>
+        <v>4.8099496310000003</v>
       </c>
       <c r="I31">
-        <v>2.349909851</v>
+        <v>1.962018209</v>
       </c>
       <c r="J31">
-        <v>2.916987491</v>
+        <v>4.8967400110000003</v>
       </c>
       <c r="K31">
-        <v>1.7118722850000001</v>
+        <v>2.870029282</v>
       </c>
       <c r="L31">
-        <v>4.5414139169999999</v>
+        <v>3.0912598509999998</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>76</v>
@@ -2331,299 +2322,299 @@
         <v>81</v>
       </c>
       <c r="E32">
-        <v>4.1500677860000001</v>
+        <v>6.8740780170000004</v>
       </c>
       <c r="F32">
-        <v>7.21392773</v>
+        <v>12.53149771</v>
       </c>
       <c r="G32">
-        <v>4.636718525</v>
+        <v>5.7276137309999999</v>
       </c>
       <c r="H32">
-        <v>4.8099496310000003</v>
+        <v>3.455545152</v>
       </c>
       <c r="I32">
-        <v>1.962018209</v>
+        <v>1.2220951579999999</v>
       </c>
       <c r="J32">
-        <v>4.8967400110000003</v>
+        <v>3.359152629</v>
       </c>
       <c r="K32">
-        <v>2.870029282</v>
+        <v>2.013346742</v>
       </c>
       <c r="L32">
-        <v>3.0912598509999998</v>
+        <v>1.445552897</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
         <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E33">
-        <v>6.8740780170000004</v>
+        <v>6.5545822649999996</v>
       </c>
       <c r="F33">
-        <v>12.53149771</v>
+        <v>11.625370029999999</v>
       </c>
       <c r="G33">
-        <v>5.7276137309999999</v>
+        <v>6.5438313050000003</v>
       </c>
       <c r="H33">
-        <v>3.455545152</v>
+        <v>5.296698202</v>
       </c>
       <c r="I33">
-        <v>1.2220951579999999</v>
+        <v>1.179691767</v>
       </c>
       <c r="J33">
-        <v>3.359152629</v>
+        <v>2.4730608200000002</v>
       </c>
       <c r="K33">
-        <v>2.013346742</v>
+        <v>1.4605253469999999</v>
       </c>
       <c r="L33">
-        <v>1.445552897</v>
+        <v>2.004496058</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
         <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E34">
-        <v>6.5545822649999996</v>
+        <v>6.1377750329999996</v>
       </c>
       <c r="F34">
-        <v>11.625370029999999</v>
+        <v>10.67580205</v>
       </c>
       <c r="G34">
-        <v>6.5438313050000003</v>
+        <v>6.1549886159999998</v>
       </c>
       <c r="H34">
-        <v>5.296698202</v>
+        <v>4.9559400650000001</v>
       </c>
       <c r="I34">
-        <v>1.179691767</v>
+        <v>1.419581132</v>
       </c>
       <c r="J34">
-        <v>2.4730608200000002</v>
+        <v>3.1786283989999999</v>
       </c>
       <c r="K34">
-        <v>1.4605253469999999</v>
+        <v>1.714438154</v>
       </c>
       <c r="L34">
-        <v>2.004496058</v>
+        <v>1.7584652519999999</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
         <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
         <v>82</v>
       </c>
       <c r="E35">
-        <v>6.1377750329999996</v>
+        <v>6.8183489499999999</v>
       </c>
       <c r="F35">
-        <v>10.67580205</v>
+        <v>12.35194675</v>
       </c>
       <c r="G35">
-        <v>6.1549886159999998</v>
+        <v>6.5759935159999996</v>
       </c>
       <c r="H35">
-        <v>4.9559400650000001</v>
+        <v>5.0703694779999999</v>
       </c>
       <c r="I35">
-        <v>1.419581132</v>
+        <v>1.1028306370000001</v>
       </c>
       <c r="J35">
-        <v>3.1786283989999999</v>
+        <v>2.3536245880000002</v>
       </c>
       <c r="K35">
-        <v>1.714438154</v>
+        <v>1.538815271</v>
       </c>
       <c r="L35">
-        <v>1.7584652519999999</v>
+        <v>1.603618336</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
         <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
         <v>82</v>
       </c>
       <c r="E36">
-        <v>6.8183489499999999</v>
+        <v>5.8660424879999997</v>
       </c>
       <c r="F36">
-        <v>12.35194675</v>
+        <v>8.3652399590000002</v>
       </c>
       <c r="G36">
-        <v>6.5759935159999996</v>
+        <v>4.4341363789999999</v>
       </c>
       <c r="H36">
-        <v>5.0703694779999999</v>
+        <v>3.7379746479999998</v>
       </c>
       <c r="I36">
-        <v>1.1028306370000001</v>
+        <v>2.0483576139999999</v>
       </c>
       <c r="J36">
-        <v>2.3536245880000002</v>
+        <v>4.6225724550000002</v>
       </c>
       <c r="K36">
-        <v>1.538815271</v>
+        <v>2.5676633099999999</v>
       </c>
       <c r="L36">
-        <v>1.603618336</v>
+        <v>1.3398333769999999</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
         <v>82</v>
       </c>
       <c r="E37">
-        <v>5.8660424879999997</v>
+        <v>6.0554723109999999</v>
       </c>
       <c r="F37">
-        <v>8.3652399590000002</v>
+        <v>10.40071783</v>
       </c>
       <c r="G37">
-        <v>4.4341363789999999</v>
+        <v>5.9347709990000004</v>
       </c>
       <c r="H37">
-        <v>3.7379746479999998</v>
+        <v>5.254195588</v>
       </c>
       <c r="I37">
-        <v>2.0483576139999999</v>
+        <v>1.3494173709999999</v>
       </c>
       <c r="J37">
-        <v>4.6225724550000002</v>
+        <v>3.1097919759999999</v>
       </c>
       <c r="K37">
-        <v>2.5676633099999999</v>
+        <v>1.8991014399999999</v>
       </c>
       <c r="L37">
-        <v>1.3398333769999999</v>
+        <v>2.1964537590000002</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
         <v>82</v>
       </c>
       <c r="E38">
-        <v>6.0554723109999999</v>
+        <v>6.3253669309999996</v>
       </c>
       <c r="F38">
-        <v>10.40071783</v>
+        <v>8.3564561220000009</v>
       </c>
       <c r="G38">
-        <v>5.9347709990000004</v>
+        <v>5.0071194549999998</v>
       </c>
       <c r="H38">
-        <v>5.254195588</v>
+        <v>4.8748799319999998</v>
       </c>
       <c r="I38">
-        <v>1.3494173709999999</v>
+        <v>1.602274746</v>
       </c>
       <c r="J38">
-        <v>3.1097919759999999</v>
+        <v>3.6174031819999999</v>
       </c>
       <c r="K38">
-        <v>1.8991014399999999</v>
+        <v>2.0698716570000002</v>
       </c>
       <c r="L38">
-        <v>2.1964537590000002</v>
+        <v>2.795979027</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
         <v>82</v>
       </c>
       <c r="E39">
-        <v>6.3253669309999996</v>
+        <v>4.9619604280000003</v>
       </c>
       <c r="F39">
-        <v>8.3564561220000009</v>
+        <v>7.6566140709999999</v>
       </c>
       <c r="G39">
-        <v>5.0071194549999998</v>
+        <v>5.0875787790000002</v>
       </c>
       <c r="H39">
-        <v>4.8748799319999998</v>
+        <v>5.5098473390000002</v>
       </c>
       <c r="I39">
-        <v>1.602274746</v>
+        <v>1.7389397900000001</v>
       </c>
       <c r="J39">
-        <v>3.6174031819999999</v>
+        <v>3.8350201209999999</v>
       </c>
       <c r="K39">
-        <v>2.0698716570000002</v>
+        <v>2.2355719440000001</v>
       </c>
       <c r="L39">
-        <v>2.795979027</v>
+        <v>3.4170729610000001</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
@@ -2635,299 +2626,299 @@
         <v>82</v>
       </c>
       <c r="E40">
-        <v>4.9619604280000003</v>
+        <v>4.2903340569999999</v>
       </c>
       <c r="F40">
-        <v>7.6566140709999999</v>
+        <v>7.0989575949999999</v>
       </c>
       <c r="G40">
-        <v>5.0875787790000002</v>
+        <v>4.9499167440000003</v>
       </c>
       <c r="H40">
-        <v>5.5098473390000002</v>
+        <v>5.6832508510000004</v>
       </c>
       <c r="I40">
-        <v>1.7389397900000001</v>
+        <v>1.847226083</v>
       </c>
       <c r="J40">
-        <v>3.8350201209999999</v>
+        <v>4.4965542650000003</v>
       </c>
       <c r="K40">
-        <v>2.2355719440000001</v>
+        <v>2.5501026699999998</v>
       </c>
       <c r="L40">
-        <v>3.4170729610000001</v>
+        <v>3.061041844</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
         <v>82</v>
       </c>
       <c r="E41">
-        <v>4.2903340569999999</v>
+        <v>4.6347662930000002</v>
       </c>
       <c r="F41">
-        <v>7.0989575949999999</v>
+        <v>7.3494934130000003</v>
       </c>
       <c r="G41">
-        <v>4.9499167440000003</v>
+        <v>5.1592278179999997</v>
       </c>
       <c r="H41">
-        <v>5.6832508510000004</v>
+        <v>5.9666219900000002</v>
       </c>
       <c r="I41">
-        <v>1.847226083</v>
+        <v>1.9178083029999999</v>
       </c>
       <c r="J41">
-        <v>4.4965542650000003</v>
+        <v>3.6386323269999998</v>
       </c>
       <c r="K41">
-        <v>2.5501026699999998</v>
+        <v>2.1759946060000002</v>
       </c>
       <c r="L41">
-        <v>3.061041844</v>
+        <v>3.7503361810000002</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
         <v>82</v>
       </c>
       <c r="E42">
-        <v>4.6347662930000002</v>
+        <v>6.193682022</v>
       </c>
       <c r="F42">
-        <v>7.3494934130000003</v>
+        <v>10.67423756</v>
       </c>
       <c r="G42">
-        <v>5.1592278179999997</v>
+        <v>5.8168924879999997</v>
       </c>
       <c r="H42">
-        <v>5.9666219900000002</v>
+        <v>4.7824848759999998</v>
       </c>
       <c r="I42">
-        <v>1.9178083029999999</v>
+        <v>1.3701030839999999</v>
       </c>
       <c r="J42">
-        <v>3.6386323269999998</v>
+        <v>3.5407270729999998</v>
       </c>
       <c r="K42">
-        <v>2.1759946060000002</v>
+        <v>1.8708525600000001</v>
       </c>
       <c r="L42">
-        <v>3.7503361810000002</v>
+        <v>1.928094414</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
         <v>82</v>
       </c>
       <c r="E43">
-        <v>6.193682022</v>
+        <v>4.7043594420000003</v>
       </c>
       <c r="F43">
-        <v>10.67423756</v>
+        <v>7.453926794</v>
       </c>
       <c r="G43">
-        <v>5.8168924879999997</v>
+        <v>5.102325928</v>
       </c>
       <c r="H43">
-        <v>4.7824848759999998</v>
+        <v>5.8746697929999998</v>
       </c>
       <c r="I43">
-        <v>1.3701030839999999</v>
+        <v>1.833700364</v>
       </c>
       <c r="J43">
-        <v>3.5407270729999998</v>
+        <v>3.5823050090000002</v>
       </c>
       <c r="K43">
-        <v>1.8708525600000001</v>
+        <v>2.0875210119999998</v>
       </c>
       <c r="L43">
-        <v>1.928094414</v>
+        <v>3.7276786710000001</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
         <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
         <v>82</v>
       </c>
       <c r="E44">
-        <v>4.7043594420000003</v>
+        <v>4.6375611130000003</v>
       </c>
       <c r="F44">
-        <v>7.453926794</v>
+        <v>7.1983465500000001</v>
       </c>
       <c r="G44">
-        <v>5.102325928</v>
+        <v>5.2962797320000004</v>
       </c>
       <c r="H44">
-        <v>5.8746697929999998</v>
+        <v>6.0743834650000004</v>
       </c>
       <c r="I44">
-        <v>1.833700364</v>
+        <v>1.7646298389999999</v>
       </c>
       <c r="J44">
-        <v>3.5823050090000002</v>
+        <v>2.9459966180000001</v>
       </c>
       <c r="K44">
-        <v>2.0875210119999998</v>
+        <v>1.8839718409999999</v>
       </c>
       <c r="L44">
-        <v>3.7276786710000001</v>
+        <v>4.9133583359999999</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
         <v>82</v>
       </c>
       <c r="E45">
-        <v>4.6375611130000003</v>
+        <v>4.8118768359999997</v>
       </c>
       <c r="F45">
-        <v>7.1983465500000001</v>
+        <v>7.5796013630000001</v>
       </c>
       <c r="G45">
-        <v>5.2962797320000004</v>
+        <v>4.752279079</v>
       </c>
       <c r="H45">
-        <v>6.0743834650000004</v>
+        <v>4.9470365740000002</v>
       </c>
       <c r="I45">
-        <v>1.7646298389999999</v>
+        <v>1.8087423010000001</v>
       </c>
       <c r="J45">
-        <v>2.9459966180000001</v>
+        <v>4.7555714120000001</v>
       </c>
       <c r="K45">
-        <v>1.8839718409999999</v>
+        <v>2.528896107</v>
       </c>
       <c r="L45">
-        <v>4.9133583359999999</v>
+        <v>2.6466059610000001</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
         <v>80</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
         <v>82</v>
       </c>
       <c r="E46">
-        <v>4.8118768359999997</v>
+        <v>4.5408480999999998</v>
       </c>
       <c r="F46">
-        <v>7.5796013630000001</v>
+        <v>7.1318284350000001</v>
       </c>
       <c r="G46">
-        <v>4.752279079</v>
+        <v>5.4196149179999997</v>
       </c>
       <c r="H46">
-        <v>4.9470365740000002</v>
+        <v>6.5055717099999999</v>
       </c>
       <c r="I46">
-        <v>1.8087423010000001</v>
+        <v>1.770509203</v>
       </c>
       <c r="J46">
-        <v>4.7555714120000001</v>
+        <v>2.8310313690000002</v>
       </c>
       <c r="K46">
-        <v>2.528896107</v>
+        <v>1.822426672</v>
       </c>
       <c r="L46">
-        <v>2.6466059610000001</v>
+        <v>5.0699275930000001</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
         <v>82</v>
       </c>
       <c r="E47">
-        <v>4.5408480999999998</v>
+        <v>4.9284076419999998</v>
       </c>
       <c r="F47">
-        <v>7.1318284350000001</v>
+        <v>8.2950367420000006</v>
       </c>
       <c r="G47">
-        <v>5.4196149179999997</v>
+        <v>4.7918540759999999</v>
       </c>
       <c r="H47">
-        <v>6.5055717099999999</v>
+        <v>4.3096250930000002</v>
       </c>
       <c r="I47">
-        <v>1.770509203</v>
+        <v>1.6734154459999999</v>
       </c>
       <c r="J47">
-        <v>2.8310313690000002</v>
+        <v>4.7085369459999997</v>
       </c>
       <c r="K47">
-        <v>1.822426672</v>
+        <v>2.9256406670000001</v>
       </c>
       <c r="L47">
-        <v>5.0699275930000001</v>
+        <v>2.25366585</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
         <v>76</v>
@@ -2939,299 +2930,299 @@
         <v>82</v>
       </c>
       <c r="E48">
-        <v>4.9284076419999998</v>
+        <v>6.500736689</v>
       </c>
       <c r="F48">
-        <v>8.2950367420000006</v>
+        <v>10.280270140000001</v>
       </c>
       <c r="G48">
-        <v>4.7918540759999999</v>
+        <v>5.3211289559999999</v>
       </c>
       <c r="H48">
-        <v>4.3096250930000002</v>
+        <v>3.9388570980000002</v>
       </c>
       <c r="I48">
-        <v>1.6734154459999999</v>
+        <v>1.4809090869999999</v>
       </c>
       <c r="J48">
-        <v>4.7085369459999997</v>
+        <v>3.9429075189999998</v>
       </c>
       <c r="K48">
-        <v>2.9256406670000001</v>
+        <v>2.1218540990000001</v>
       </c>
       <c r="L48">
-        <v>2.25366585</v>
+        <v>1.755792832</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
         <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
         <v>82</v>
       </c>
       <c r="E49">
-        <v>6.500736689</v>
+        <v>6.8879496739999997</v>
       </c>
       <c r="F49">
-        <v>10.280270140000001</v>
+        <v>11.51019367</v>
       </c>
       <c r="G49">
-        <v>5.3211289559999999</v>
+        <v>6.163727465</v>
       </c>
       <c r="H49">
-        <v>3.9388570980000002</v>
+        <v>4.6959922169999997</v>
       </c>
       <c r="I49">
-        <v>1.4809090869999999</v>
+        <v>1.2487903600000001</v>
       </c>
       <c r="J49">
-        <v>3.9429075189999998</v>
+        <v>2.6398193569999999</v>
       </c>
       <c r="K49">
-        <v>2.1218540990000001</v>
+        <v>1.5667244060000001</v>
       </c>
       <c r="L49">
-        <v>1.755792832</v>
+        <v>1.9305544699999999</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
         <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E50">
-        <v>6.8879496739999997</v>
+        <v>5.0759119259999999</v>
       </c>
       <c r="F50">
-        <v>11.51019367</v>
+        <v>8.1592176980000009</v>
       </c>
       <c r="G50">
-        <v>6.163727465</v>
+        <v>4.7251256860000002</v>
       </c>
       <c r="H50">
-        <v>4.6959922169999997</v>
+        <v>4.2364288239999999</v>
       </c>
       <c r="I50">
-        <v>1.2487903600000001</v>
+        <v>1.7158212850000001</v>
       </c>
       <c r="J50">
-        <v>2.6398193569999999</v>
+        <v>5.2449190999999997</v>
       </c>
       <c r="K50">
-        <v>1.5667244060000001</v>
+        <v>2.6978103330000001</v>
       </c>
       <c r="L50">
-        <v>1.9305544699999999</v>
+        <v>2.1702841149999998</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D51" t="s">
         <v>83</v>
       </c>
       <c r="E51">
-        <v>5.0759119259999999</v>
+        <v>6.384827188</v>
       </c>
       <c r="F51">
-        <v>8.1592176980000009</v>
+        <v>10.387864029999999</v>
       </c>
       <c r="G51">
-        <v>4.7251256860000002</v>
+        <v>5.6307016230000002</v>
       </c>
       <c r="H51">
-        <v>4.2364288239999999</v>
+        <v>4.3697283450000004</v>
       </c>
       <c r="I51">
-        <v>1.7158212850000001</v>
+        <v>1.485439626</v>
       </c>
       <c r="J51">
-        <v>5.2449190999999997</v>
+        <v>3.1736990490000001</v>
       </c>
       <c r="K51">
-        <v>2.6978103330000001</v>
+        <v>1.7353203319999999</v>
       </c>
       <c r="L51">
-        <v>2.1702841149999998</v>
+        <v>2.1770199670000001</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
         <v>83</v>
       </c>
       <c r="E52">
-        <v>6.384827188</v>
+        <v>6.7640376169999996</v>
       </c>
       <c r="F52">
-        <v>10.387864029999999</v>
+        <v>9.3054765610000008</v>
       </c>
       <c r="G52">
-        <v>5.6307016230000002</v>
+        <v>4.9698261170000002</v>
       </c>
       <c r="H52">
-        <v>4.3697283450000004</v>
+        <v>3.8279727970000001</v>
       </c>
       <c r="I52">
-        <v>1.485439626</v>
+        <v>1.429795511</v>
       </c>
       <c r="J52">
-        <v>3.1736990490000001</v>
+        <v>4.4199626250000001</v>
       </c>
       <c r="K52">
-        <v>1.7353203319999999</v>
+        <v>2.2846937139999999</v>
       </c>
       <c r="L52">
-        <v>2.1770199670000001</v>
+        <v>1.839654825</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D53" t="s">
         <v>83</v>
       </c>
       <c r="E53">
-        <v>6.7640376169999996</v>
+        <v>7.5711996160000004</v>
       </c>
       <c r="F53">
-        <v>9.3054765610000008</v>
+        <v>13.7424309</v>
       </c>
       <c r="G53">
-        <v>4.9698261170000002</v>
+        <v>6.7388574969999997</v>
       </c>
       <c r="H53">
-        <v>3.8279727970000001</v>
+        <v>5.342189758</v>
       </c>
       <c r="I53">
-        <v>1.429795511</v>
+        <v>0.85029698200000003</v>
       </c>
       <c r="J53">
-        <v>4.4199626250000001</v>
+        <v>1.8614065740000001</v>
       </c>
       <c r="K53">
-        <v>2.2846937139999999</v>
+        <v>1.2776732500000001</v>
       </c>
       <c r="L53">
-        <v>1.839654825</v>
+        <v>1.4501613790000001</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
         <v>83</v>
       </c>
       <c r="E54">
-        <v>7.5711996160000004</v>
+        <v>5.6862755009999999</v>
       </c>
       <c r="F54">
-        <v>13.7424309</v>
+        <v>8.451898753</v>
       </c>
       <c r="G54">
-        <v>6.7388574969999997</v>
+        <v>5.0174582069999998</v>
       </c>
       <c r="H54">
-        <v>5.342189758</v>
+        <v>4.9373150570000002</v>
       </c>
       <c r="I54">
-        <v>0.85029698200000003</v>
+        <v>1.6140583390000001</v>
       </c>
       <c r="J54">
-        <v>1.8614065740000001</v>
+        <v>3.8721185939999998</v>
       </c>
       <c r="K54">
-        <v>1.2776732500000001</v>
+        <v>2.233135034</v>
       </c>
       <c r="L54">
-        <v>1.4501613790000001</v>
+        <v>3.0154021370000001</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D55" t="s">
         <v>83</v>
       </c>
       <c r="E55">
-        <v>5.6862755009999999</v>
+        <v>6.8192866219999999</v>
       </c>
       <c r="F55">
-        <v>8.451898753</v>
+        <v>9.3658915579999995</v>
       </c>
       <c r="G55">
-        <v>5.0174582069999998</v>
+        <v>4.9789192529999999</v>
       </c>
       <c r="H55">
-        <v>4.9373150570000002</v>
+        <v>4.6957270260000001</v>
       </c>
       <c r="I55">
-        <v>1.6140583390000001</v>
+        <v>1.774494019</v>
       </c>
       <c r="J55">
-        <v>3.8721185939999998</v>
+        <v>3.4230415999999999</v>
       </c>
       <c r="K55">
-        <v>2.233135034</v>
+        <v>1.9080425050000001</v>
       </c>
       <c r="L55">
-        <v>3.0154021370000001</v>
+        <v>2.797805307</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
@@ -3243,299 +3234,299 @@
         <v>83</v>
       </c>
       <c r="E56">
-        <v>6.8192866219999999</v>
+        <v>4.8207532320000004</v>
       </c>
       <c r="F56">
-        <v>9.3658915579999995</v>
+        <v>7.3504001360000002</v>
       </c>
       <c r="G56">
-        <v>4.9789192529999999</v>
+        <v>5.3587164439999997</v>
       </c>
       <c r="H56">
-        <v>4.6957270260000001</v>
+        <v>6.2240142199999999</v>
       </c>
       <c r="I56">
-        <v>1.774494019</v>
+        <v>1.9245888280000001</v>
       </c>
       <c r="J56">
-        <v>3.4230415999999999</v>
+        <v>3.1316291459999999</v>
       </c>
       <c r="K56">
-        <v>1.9080425050000001</v>
+        <v>1.8679334970000001</v>
       </c>
       <c r="L56">
-        <v>2.797805307</v>
+        <v>4.3173309250000003</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
         <v>80</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D57" t="s">
         <v>83</v>
       </c>
       <c r="E57">
-        <v>4.8207532320000004</v>
+        <v>5.161163911</v>
       </c>
       <c r="F57">
-        <v>7.3504001360000002</v>
+        <v>7.6872605529999998</v>
       </c>
       <c r="G57">
-        <v>5.3587164439999997</v>
+        <v>5.0276901790000004</v>
       </c>
       <c r="H57">
-        <v>6.2240142199999999</v>
+        <v>5.5556918619999998</v>
       </c>
       <c r="I57">
-        <v>1.9245888280000001</v>
+        <v>1.704486038</v>
       </c>
       <c r="J57">
-        <v>3.1316291459999999</v>
+        <v>3.790218598</v>
       </c>
       <c r="K57">
-        <v>1.8679334970000001</v>
+        <v>2.2568143759999999</v>
       </c>
       <c r="L57">
-        <v>4.3173309250000003</v>
+        <v>3.3203880909999999</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
         <v>83</v>
       </c>
       <c r="E58">
-        <v>5.161163911</v>
+        <v>6.565898732</v>
       </c>
       <c r="F58">
-        <v>7.6872605529999998</v>
+        <v>10.884544679999999</v>
       </c>
       <c r="G58">
-        <v>5.0276901790000004</v>
+        <v>5.7679864820000004</v>
       </c>
       <c r="H58">
-        <v>5.5556918619999998</v>
+        <v>4.6520679129999998</v>
       </c>
       <c r="I58">
-        <v>1.704486038</v>
+        <v>1.3853607020000001</v>
       </c>
       <c r="J58">
-        <v>3.790218598</v>
+        <v>3.3273187630000001</v>
       </c>
       <c r="K58">
-        <v>2.2568143759999999</v>
+        <v>1.885292738</v>
       </c>
       <c r="L58">
-        <v>3.3203880909999999</v>
+        <v>1.572700805</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D59" t="s">
         <v>83</v>
       </c>
       <c r="E59">
-        <v>6.565898732</v>
+        <v>5.1042588200000001</v>
       </c>
       <c r="F59">
-        <v>10.884544679999999</v>
+        <v>7.32529246</v>
       </c>
       <c r="G59">
-        <v>5.7679864820000004</v>
+        <v>4.6136867370000001</v>
       </c>
       <c r="H59">
-        <v>4.6520679129999998</v>
+        <v>4.9273232800000004</v>
       </c>
       <c r="I59">
-        <v>1.3853607020000001</v>
+        <v>1.741873215</v>
       </c>
       <c r="J59">
-        <v>3.3273187630000001</v>
+        <v>4.3332719690000001</v>
       </c>
       <c r="K59">
-        <v>1.885292738</v>
+        <v>2.1994755060000002</v>
       </c>
       <c r="L59">
-        <v>1.572700805</v>
+        <v>3.5991716920000001</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
         <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D60" t="s">
         <v>83</v>
       </c>
       <c r="E60">
-        <v>5.1042588200000001</v>
+        <v>6.366301429</v>
       </c>
       <c r="F60">
-        <v>7.32529246</v>
+        <v>8.9175370909999998</v>
       </c>
       <c r="G60">
-        <v>4.6136867370000001</v>
+        <v>4.8036446030000004</v>
       </c>
       <c r="H60">
-        <v>4.9273232800000004</v>
+        <v>4.7471813110000003</v>
       </c>
       <c r="I60">
-        <v>1.741873215</v>
+        <v>1.7508739900000001</v>
       </c>
       <c r="J60">
-        <v>4.3332719690000001</v>
+        <v>3.4153489879999999</v>
       </c>
       <c r="K60">
-        <v>2.1994755060000002</v>
+        <v>2.0730652580000002</v>
       </c>
       <c r="L60">
-        <v>3.5991716920000001</v>
+        <v>3.134183894</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D61" t="s">
         <v>83</v>
       </c>
       <c r="E61">
-        <v>6.366301429</v>
+        <v>4.5887894319999996</v>
       </c>
       <c r="F61">
-        <v>8.9175370909999998</v>
+        <v>7.2311044029999998</v>
       </c>
       <c r="G61">
-        <v>4.8036446030000004</v>
+        <v>5.0821853780000001</v>
       </c>
       <c r="H61">
-        <v>4.7471813110000003</v>
+        <v>5.8004908860000004</v>
       </c>
       <c r="I61">
-        <v>1.7508739900000001</v>
+        <v>1.8224741659999999</v>
       </c>
       <c r="J61">
-        <v>3.4153489879999999</v>
+        <v>3.8933177539999999</v>
       </c>
       <c r="K61">
-        <v>2.0730652580000002</v>
+        <v>2.2282765160000002</v>
       </c>
       <c r="L61">
-        <v>3.134183894</v>
+        <v>3.7212168320000001</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
         <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D62" t="s">
         <v>83</v>
       </c>
       <c r="E62">
-        <v>4.5887894319999996</v>
+        <v>6.8731498259999997</v>
       </c>
       <c r="F62">
-        <v>7.2311044029999998</v>
+        <v>8.7269744350000007</v>
       </c>
       <c r="G62">
-        <v>5.0821853780000001</v>
+        <v>5.0461563710000004</v>
       </c>
       <c r="H62">
-        <v>5.8004908860000004</v>
+        <v>4.7239159309999996</v>
       </c>
       <c r="I62">
-        <v>1.8224741659999999</v>
+        <v>1.411051348</v>
       </c>
       <c r="J62">
-        <v>3.8933177539999999</v>
+        <v>3.1344561089999998</v>
       </c>
       <c r="K62">
-        <v>2.2282765160000002</v>
+        <v>1.9426256070000001</v>
       </c>
       <c r="L62">
-        <v>3.7212168320000001</v>
+        <v>3.3368577770000001</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
         <v>83</v>
       </c>
       <c r="E63">
-        <v>6.8731498259999997</v>
+        <v>7.0750001549999997</v>
       </c>
       <c r="F63">
-        <v>8.7269744350000007</v>
+        <v>10.970013440000001</v>
       </c>
       <c r="G63">
-        <v>5.0461563710000004</v>
+        <v>5.4168556370000003</v>
       </c>
       <c r="H63">
-        <v>4.7239159309999996</v>
+        <v>4.2302959160000002</v>
       </c>
       <c r="I63">
-        <v>1.411051348</v>
+        <v>1.4508903580000001</v>
       </c>
       <c r="J63">
-        <v>3.1344561089999998</v>
+        <v>2.874393575</v>
       </c>
       <c r="K63">
-        <v>1.9426256070000001</v>
+        <v>1.6350837119999999</v>
       </c>
       <c r="L63">
-        <v>3.3368577770000001</v>
+        <v>2.2037279399999998</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
         <v>76</v>
@@ -3547,108 +3538,70 @@
         <v>83</v>
       </c>
       <c r="E64">
-        <v>7.0750001549999997</v>
+        <v>8.5255934619999998</v>
       </c>
       <c r="F64">
-        <v>10.970013440000001</v>
+        <v>12.0174714</v>
       </c>
       <c r="G64">
-        <v>5.4168556370000003</v>
+        <v>5.7682333359999998</v>
       </c>
       <c r="H64">
-        <v>4.2302959160000002</v>
+        <v>4.1965145450000003</v>
       </c>
       <c r="I64">
-        <v>1.4508903580000001</v>
+        <v>1.0613623969999999</v>
       </c>
       <c r="J64">
-        <v>2.874393575</v>
+        <v>2.554588785</v>
       </c>
       <c r="K64">
-        <v>1.6350837119999999</v>
+        <v>1.5120676790000001</v>
       </c>
       <c r="L64">
-        <v>2.2037279399999998</v>
+        <v>1.410549058</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
         <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
         <v>83</v>
       </c>
       <c r="E65">
-        <v>8.5255934619999998</v>
+        <v>8.3416168759999998</v>
       </c>
       <c r="F65">
-        <v>12.0174714</v>
+        <v>12.481709929999999</v>
       </c>
       <c r="G65">
-        <v>5.7682333359999998</v>
+        <v>6.2383198049999997</v>
       </c>
       <c r="H65">
-        <v>4.1965145450000003</v>
+        <v>4.6556274889999996</v>
       </c>
       <c r="I65">
-        <v>1.0613623969999999</v>
+        <v>0.92265952299999998</v>
       </c>
       <c r="J65">
-        <v>2.554588785</v>
+        <v>2.1727876529999999</v>
       </c>
       <c r="K65">
-        <v>1.5120676790000001</v>
+        <v>1.268195228</v>
       </c>
       <c r="L65">
-        <v>1.410549058</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" t="s">
-        <v>77</v>
-      </c>
-      <c r="D66" t="s">
-        <v>83</v>
-      </c>
-      <c r="E66">
-        <v>8.3416168759999998</v>
-      </c>
-      <c r="F66">
-        <v>12.481709929999999</v>
-      </c>
-      <c r="G66">
-        <v>6.2383198049999997</v>
-      </c>
-      <c r="H66">
-        <v>4.6556274889999996</v>
-      </c>
-      <c r="I66">
-        <v>0.92265952299999998</v>
-      </c>
-      <c r="J66">
-        <v>2.1727876529999999</v>
-      </c>
-      <c r="K66">
-        <v>1.268195228</v>
-      </c>
-      <c r="L66">
         <v>1.735912761</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D2:D66" xr:uid="{9C183A2B-4849-EF46-B989-08825FB4A4F5}"/>
+  <autoFilter ref="D1:D65" xr:uid="{9C183A2B-4849-EF46-B989-08825FB4A4F5}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>